<commit_message>
TradingModel_v2 - 2021/11/17 data updated
</commit_message>
<xml_diff>
--- a/TradingModel_TotalCapital.xlsx
+++ b/TradingModel_TotalCapital.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -517,11 +517,19 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="3" t="n">
+      <c r="A10" s="2" t="n">
         <v>44516</v>
       </c>
       <c r="B10" t="n">
         <v>71823.60000000001</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="n">
+        <v>44517</v>
+      </c>
+      <c r="B11" t="n">
+        <v>66336.55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TradingModel_v2 - 2021/11/18 data updated
</commit_message>
<xml_diff>
--- a/TradingModel_TotalCapital.xlsx
+++ b/TradingModel_TotalCapital.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -525,11 +525,19 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="3" t="n">
+      <c r="A11" s="2" t="n">
         <v>44517</v>
       </c>
       <c r="B11" t="n">
         <v>66336.55</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="n">
+        <v>44518</v>
+      </c>
+      <c r="B12" t="n">
+        <v>65081.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TradingModel_v2 - 2021/11/19 data updated
</commit_message>
<xml_diff>
--- a/TradingModel_TotalCapital.xlsx
+++ b/TradingModel_TotalCapital.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -533,11 +533,19 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="3" t="n">
+      <c r="A12" s="2" t="n">
         <v>44518</v>
       </c>
       <c r="B12" t="n">
         <v>65081.4</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="n">
+        <v>44519</v>
+      </c>
+      <c r="B13" t="n">
+        <v>61854.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TradingModel_v2 - 2021/11/22 data updated
</commit_message>
<xml_diff>
--- a/TradingModel_TotalCapital.xlsx
+++ b/TradingModel_TotalCapital.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -541,11 +541,19 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="3" t="n">
+      <c r="A13" s="2" t="n">
         <v>44519</v>
       </c>
       <c r="B13" t="n">
         <v>61854.9</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="n">
+        <v>44522</v>
+      </c>
+      <c r="B14" t="n">
+        <v>63372.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TradingModel_v2 - 2021/11/23 data updated
</commit_message>
<xml_diff>
--- a/TradingModel_TotalCapital.xlsx
+++ b/TradingModel_TotalCapital.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -549,11 +549,19 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="3" t="n">
+      <c r="A14" s="2" t="n">
         <v>44522</v>
       </c>
       <c r="B14" t="n">
         <v>63372.8</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="n">
+        <v>44523</v>
+      </c>
+      <c r="B15" t="n">
+        <v>60340.15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2021/11/26 data updated / 部份平倉損益更正
</commit_message>
<xml_diff>
--- a/TradingModel_TotalCapital.xlsx
+++ b/TradingModel_TotalCapital.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -573,11 +573,19 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="3" t="n">
+      <c r="A17" s="2" t="n">
         <v>44525</v>
       </c>
       <c r="B17" t="n">
         <v>61790.05</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="3" t="n">
+        <v>44526</v>
+      </c>
+      <c r="B18" t="n">
+        <v>65265.85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>